<commit_message>
Added Matlab UC simulation files.
</commit_message>
<xml_diff>
--- a/input_files/UC_case_study_simple_network_A.xlsx
+++ b/input_files/UC_case_study_simple_network_A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bus index" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>From Index</t>
   </si>
@@ -126,36 +126,12 @@
     <t>Utility storage efficiency</t>
   </si>
   <si>
-    <t>Wind</t>
-  </si>
-  <si>
     <t>Gainsboro</t>
   </si>
   <si>
-    <t>ForestGreen</t>
-  </si>
-  <si>
-    <t>Rooftop PV</t>
-  </si>
-  <si>
     <t>DimGray</t>
   </si>
   <si>
-    <t>Bubble MUN Wind 2014-2045_0910refyr.csv</t>
-  </si>
-  <si>
-    <t>SWNSW Solar Real PV.csv</t>
-  </si>
-  <si>
-    <t>This example uses NSW only, so only 1 region (node) is specified</t>
-  </si>
-  <si>
-    <t>The maximum demand for this example is 12979 MW on Friday 22 Jan at 3pm</t>
-  </si>
-  <si>
-    <t>Transmission line series reactance set to limit voltage angle to 30 degrees</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
@@ -169,6 +145,69 @@
   </si>
   <si>
     <t>CSP &amp; PV solar multiple</t>
+  </si>
+  <si>
+    <t>NNS Solar PV.csv</t>
+  </si>
+  <si>
+    <t>Bubble SWQ Wind 2014-2045_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>Bubble SEV Wind 2014-2045_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>LV Solar Real PV.csv</t>
+  </si>
+  <si>
+    <t>2014 QLD1 Medium 10POE_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>2014 SA1 Medium 10POE_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>2014 VIC1 Medium 10POE_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>Moccasin</t>
+  </si>
+  <si>
+    <t>Khaki</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Rooftop PV NSW</t>
+  </si>
+  <si>
+    <t>Rooftop PV VIC</t>
+  </si>
+  <si>
+    <t>Rooftop PV QLD</t>
+  </si>
+  <si>
+    <t>Rooftop PV SA</t>
+  </si>
+  <si>
+    <t>Bubble SEN Wind 2014-2045_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>Bubble NEN Wind 2014-2045_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>CAN Solar PV.csv</t>
+  </si>
+  <si>
+    <t>SWQ Solar PV.csv</t>
+  </si>
+  <si>
+    <t>ADE Solar Real PV.csv</t>
+  </si>
+  <si>
+    <t>Bubble FLS Wind 2014-2045_0910refyr.csv</t>
+  </si>
+  <si>
+    <t>Node 2 includes busses 1 &amp; 2 (node numbering chosen to match bus numbers for simplicity)</t>
   </si>
 </sst>
 </file>
@@ -249,7 +288,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="591">
+  <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -841,13 +880,82 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -868,15 +976,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="591">
+  <cellStyles count="663">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1172,6 +1277,42 @@
     <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="650" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="652" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="654" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="656" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1467,6 +1608,42 @@
     <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="649" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="651" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="653" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="655" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1804,13 +1981,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="36.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="36.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="58.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1829,91 +2006,93 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6">
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>40</v>
+      <c r="D2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>40</v>
+      <c r="D3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>40</v>
+      <c r="D4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>40</v>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>40</v>
+      <c r="D6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1929,24 +2108,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="28" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1967,107 +2146,149 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>4</v>
-      </c>
-      <c r="C2" s="11">
-        <f>(PI()/6)/(E2/100)*D2</f>
-        <v>6.5449846949787354E-3</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9">
+        <f t="shared" ref="C2:C8" si="0">(PI()/6)/(E2/100)*D2</f>
+        <v>1.4959965017094252E-2</v>
+      </c>
+      <c r="D2" s="5">
         <v>1</v>
       </c>
-      <c r="E2" s="6">
-        <v>8000</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="E2" s="5">
+        <v>3500</v>
+      </c>
+      <c r="F2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
         <v>3</v>
       </c>
-      <c r="C3" s="11">
-        <f t="shared" ref="C3:C5" si="0">(PI()/6)/(E3/100)*D3</f>
-        <v>0.10471975511965977</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="9">
+        <f t="shared" si="0"/>
+        <v>1.4959965017094252E-2</v>
+      </c>
+      <c r="D3" s="5">
         <v>1</v>
       </c>
-      <c r="E3" s="6">
-        <v>500</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="5">
+        <v>3500</v>
+      </c>
+      <c r="F3" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="6">
-        <v>4</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9">
         <f t="shared" si="0"/>
-        <v>8.7266462599716477E-3</v>
-      </c>
-      <c r="D4" s="6">
+        <v>1.8699956271367814E-2</v>
+      </c>
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
-        <v>6000</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
+        <v>2800</v>
+      </c>
+      <c r="F4" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
         <v>4</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="9">
         <f t="shared" si="0"/>
-        <v>0.10471975511965977</v>
-      </c>
-      <c r="D5" s="6">
+        <v>2.0943951023931952E-2</v>
+      </c>
+      <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="6">
-        <v>500</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E5" s="5">
+        <v>2500</v>
+      </c>
+      <c r="F5" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>1.0471975511965976E-2</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3089969389957471E-2</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>4000</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C6" s="11">
-        <f>(PI()/6)/(E6/100)*D6</f>
-        <v>7.4799825085471259E-3</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2</v>
-      </c>
-      <c r="E6" s="6">
-        <v>14000</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1635528346628862E-2</v>
+      </c>
+      <c r="D8" s="5">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>4500</v>
+      </c>
+      <c r="F8" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2086,19 +2307,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32" style="3" customWidth="1"/>
-    <col min="6" max="6" width="66" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32" style="2" customWidth="1"/>
+    <col min="6" max="6" width="76" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2122,51 +2343,75 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="5">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>41</v>
+      <c r="C2" s="5">
+        <v>0.2555</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="10" t="s">
-        <v>42</v>
+      <c r="A3" s="5">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.36980000000000002</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10" t="s">
-        <v>43</v>
+      <c r="A4" s="5">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.1636</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.21110000000000001</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2181,288 +2426,226 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="46.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="40.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="18.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="46.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="40.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="39.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" s="8" t="s">
+      <c r="O1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="8" t="s">
-        <v>48</v>
+      <c r="T1" s="7" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="D2" s="5">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5">
+        <v>20000</v>
+      </c>
+      <c r="F2" s="5">
+        <f>0.35*E2</f>
+        <v>7000</v>
+      </c>
+      <c r="G2" s="5">
+        <f>0.4*E2</f>
         <v>8000</v>
       </c>
-      <c r="F2" s="6">
-        <f>0.4*E2</f>
-        <v>3200</v>
-      </c>
-      <c r="G2" s="6">
-        <v>150</v>
-      </c>
-      <c r="H2" s="6">
-        <v>100</v>
-      </c>
-      <c r="I2" s="6">
+      <c r="H2" s="5">
+        <f>G2</f>
+        <v>8000</v>
+      </c>
+      <c r="I2" s="5">
         <v>1050</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
         <v>0</v>
       </c>
-      <c r="K2" s="6">
-        <v>7.14</v>
-      </c>
-      <c r="L2" s="6">
+      <c r="K2" s="5">
+        <v>20</v>
+      </c>
+      <c r="L2" s="5">
         <v>16</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>16</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="5">
         <v>0</v>
       </c>
-      <c r="P2" s="6">
+      <c r="P2" s="5">
         <v>0</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="5">
         <v>0</v>
       </c>
-      <c r="R2" s="6">
+      <c r="R2" s="5">
         <v>0</v>
       </c>
-      <c r="S2" s="6">
+      <c r="S2" s="5">
         <v>0</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5">
         <v>3</v>
       </c>
-      <c r="E3" s="6">
-        <v>6500</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="5">
+        <v>15000</v>
+      </c>
+      <c r="F3" s="5">
+        <f>0.02*E3</f>
+        <v>300</v>
+      </c>
+      <c r="G3" s="5">
+        <f>3*E3</f>
+        <v>45000</v>
+      </c>
+      <c r="H3" s="5">
+        <f>G3</f>
+        <v>45000</v>
+      </c>
+      <c r="I3" s="5">
+        <v>700</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
         <v>100</v>
       </c>
-      <c r="G3" s="6">
-        <f>0.9*E3</f>
-        <v>5850</v>
-      </c>
-      <c r="H3" s="6">
-        <f>G3</f>
-        <v>5850</v>
-      </c>
-      <c r="I3" s="6">
-        <v>700</v>
-      </c>
-      <c r="J3" s="6">
+      <c r="L3" s="5">
+        <v>1</v>
+      </c>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="6">
-        <v>25.61</v>
-      </c>
-      <c r="L3" s="6">
-        <v>16</v>
-      </c>
-      <c r="M3" s="6">
-        <v>16</v>
-      </c>
-      <c r="N3" s="6">
+      <c r="O3" s="5">
         <v>0</v>
       </c>
-      <c r="O3" s="6">
+      <c r="P3" s="5">
         <v>0</v>
       </c>
-      <c r="P3" s="6">
+      <c r="Q3" s="5">
         <v>0</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="R3" s="5">
         <v>0</v>
       </c>
-      <c r="R3" s="6">
+      <c r="S3" s="5">
         <v>0</v>
       </c>
-      <c r="S3" s="6">
-        <v>0</v>
-      </c>
-      <c r="T3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="6">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1000</v>
-      </c>
-      <c r="F4" s="6">
-        <f>E4*0.05</f>
-        <v>50</v>
-      </c>
-      <c r="G4" s="6">
-        <f>0.9*E4</f>
-        <v>900</v>
-      </c>
-      <c r="H4" s="6">
-        <f>G4</f>
-        <v>900</v>
-      </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>3.86</v>
-      </c>
-      <c r="L4" s="6">
-        <v>0</v>
-      </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0</v>
-      </c>
-      <c r="S4" s="6">
-        <v>0</v>
-      </c>
-      <c r="T4" s="6">
+      <c r="T3" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>